<commit_message>
fix project births format to Number-automatic (though  shouldn't be necessary)
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Kenya/Input_Kenya_2016.xlsx
+++ b/input_spreadsheets/Kenya/Input_Kenya_2016.xlsx
@@ -326,11 +326,7 @@
     </font>
     <font/>
     <font>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
+      <sz val="10.0"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -340,6 +336,9 @@
     </font>
     <font>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -379,22 +378,22 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="10" xfId="0" applyFont="1" applyNumberFormat="1"/>
@@ -402,34 +401,34 @@
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="2" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -438,29 +437,29 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1599,7 +1598,7 @@
       </c>
       <c r="B3" s="8" t="str">
         <f t="shared" ref="B3:B15" si="1">$B2*1.028</f>
-        <v>2,201,936</v>
+        <v>2201936</v>
       </c>
     </row>
     <row r="4">
@@ -1608,7 +1607,7 @@
       </c>
       <c r="B4" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>2,263,590</v>
+        <v>2263590</v>
       </c>
     </row>
     <row r="5">
@@ -1617,7 +1616,7 @@
       </c>
       <c r="B5" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>2,326,971</v>
+        <v>2326971</v>
       </c>
     </row>
     <row r="6">
@@ -1626,7 +1625,7 @@
       </c>
       <c r="B6" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>2,392,126</v>
+        <v>2392126</v>
       </c>
     </row>
     <row r="7">
@@ -1635,7 +1634,7 @@
       </c>
       <c r="B7" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>2,459,105</v>
+        <v>2459105</v>
       </c>
     </row>
     <row r="8">
@@ -1644,7 +1643,7 @@
       </c>
       <c r="B8" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>2,527,960</v>
+        <v>2527960</v>
       </c>
     </row>
     <row r="9">
@@ -1653,7 +1652,7 @@
       </c>
       <c r="B9" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>2,598,743</v>
+        <v>2598743</v>
       </c>
     </row>
     <row r="10">
@@ -1662,7 +1661,7 @@
       </c>
       <c r="B10" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>2,671,508</v>
+        <v>2671508</v>
       </c>
     </row>
     <row r="11">
@@ -1671,7 +1670,7 @@
       </c>
       <c r="B11" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>2,746,310</v>
+        <v>2746310</v>
       </c>
     </row>
     <row r="12">
@@ -1680,7 +1679,7 @@
       </c>
       <c r="B12" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>2,823,207</v>
+        <v>2823207</v>
       </c>
     </row>
     <row r="13">
@@ -1689,7 +1688,7 @@
       </c>
       <c r="B13" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>2,902,257</v>
+        <v>2902257</v>
       </c>
     </row>
     <row r="14">
@@ -1698,7 +1697,7 @@
       </c>
       <c r="B14" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>2,983,520</v>
+        <v>2983520</v>
       </c>
     </row>
     <row r="15">
@@ -1707,7 +1706,7 @@
       </c>
       <c r="B15" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>3,067,058</v>
+        <v>3067058</v>
       </c>
     </row>
     <row r="16">

</xml_diff>